<commit_message>
Issue #15: Fix broken Drools tests.
</commit_message>
<xml_diff>
--- a/mdw-workflow/assets/com/centurylink/mdw/tests/workflow/drools-multiSheetDecisionTable.xlsx
+++ b/mdw-workflow/assets/com/centurylink/mdw/tests/workflow/drools-multiSheetDecisionTable.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="11445" windowHeight="3915"/>
@@ -127,14 +127,14 @@
     <t>Order Routing Decision Table -- North/South</t>
   </si>
   <si>
-    <t>java.util.Map, java.util.Date, com.centurylink.mdw.workflow.activity.rules.DroolsActivity</t>
+    <t>java.util.Map, java.util.Date, com.centurylink.mdw.drools.DroolsActivity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -384,8 +384,41 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -464,6 +497,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -498,6 +532,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -673,14 +708,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
@@ -689,12 +724,12 @@
     <col min="5" max="5" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
         <v>0</v>
@@ -705,7 +740,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
@@ -716,7 +751,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -727,7 +762,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
         <v>5</v>
@@ -736,7 +771,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="4" t="s">
         <v>6</v>
@@ -751,7 +786,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
         <v>21</v>
@@ -762,7 +797,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="4" t="s">
         <v>13</v>
@@ -777,7 +812,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>11</v>
       </c>
@@ -794,7 +829,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="16" t="s">
         <v>30</v>
@@ -809,7 +844,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="17"/>
       <c r="C13" s="5" t="s">
@@ -820,7 +855,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="16" t="s">
         <v>31</v>
@@ -835,7 +870,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="17"/>
       <c r="C15" s="9" t="s">
@@ -846,21 +881,21 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="10"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="10"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="2" t="s">
         <v>14</v>
@@ -884,14 +919,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
@@ -900,12 +935,12 @@
     <col min="5" max="5" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
         <v>0</v>
@@ -916,7 +951,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
@@ -927,7 +962,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -938,7 +973,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
         <v>5</v>
@@ -947,7 +982,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="4" t="s">
         <v>6</v>
@@ -962,7 +997,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
         <v>21</v>
@@ -973,7 +1008,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="4" t="s">
         <v>13</v>
@@ -988,7 +1023,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>11</v>
       </c>
@@ -1005,7 +1040,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="16" t="s">
         <v>8</v>
@@ -1020,7 +1055,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="17"/>
       <c r="C13" s="5" t="s">
@@ -1031,7 +1066,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="16" t="s">
         <v>9</v>
@@ -1046,7 +1081,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="17"/>
       <c r="C15" s="9" t="s">
@@ -1057,21 +1092,21 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="10"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="10"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="2" t="s">
         <v>14</v>
@@ -1095,26 +1130,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>